<commit_message>
anhht - refactor API uploadExcel đvhc, thêm API upload excel user, refactor DVHCId => DVHCCode
</commit_message>
<xml_diff>
--- a/aspnet-core/src/KiemKeDatDai.Web.Host/wwwroot/Templates/excels/TemplateImport_DVHC.xlsx
+++ b/aspnet-core/src/KiemKeDatDai.Web.Host/wwwroot/Templates/excels/TemplateImport_DVHC.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Huy\Coder\Projects\OutSources\KiemKeDatDai\aspnet-core\src\KiemKeDatDai.Web.Host\wwwroot\Templates\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\word\KiemKeDatDai2024\aspnet-core\src\KiemKeDatDai.Web.Host\wwwroot\Templates\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9982705-3478-4EE3-B674-1EDEA3C20B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7480" windowHeight="2830"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>TenVung</t>
   </si>
@@ -48,17 +49,23 @@
   </si>
   <si>
     <t>MaXa</t>
+  </si>
+  <si>
+    <t>CapDvhc</t>
+  </si>
+  <si>
+    <t>Nam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -87,7 +94,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -103,17 +110,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:H1048576"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="TenVung" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="MaVung" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="TenTinh" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="MaTinh" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="TenHuyen" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="MaHuyen" dataCellStyle="Normal"/>
-    <tableColumn id="7" name="TenXa" dataCellStyle="Normal"/>
-    <tableColumn id="8" name="MaXa" dataCellStyle="Normal"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J1048575" totalsRowShown="0">
+  <autoFilter ref="A1:J1048575" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TenVung"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="MaVung"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TenTinh"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MaTinh"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TenHuyen"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="MaHuyen"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="TenXa"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="MaXa"/>
+    <tableColumn id="9" xr3:uid="{CD680343-7F2A-43C0-B945-0B37D4029135}" name="CapDvhc"/>
+    <tableColumn id="10" xr3:uid="{EB7F835A-183B-4780-99EF-DA7C956C13CB}" name="Nam"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -381,26 +390,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" customWidth="1"/>
-    <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.875" customWidth="1"/>
+    <col min="8" max="8" width="8.375" customWidth="1"/>
+    <col min="9" max="9" width="20.875" customWidth="1"/>
+    <col min="10" max="10" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,31 +436,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>